<commit_message>
Lists page basics are down. You can add new list
</commit_message>
<xml_diff>
--- a/Taskr_gantt.xlsx
+++ b/Taskr_gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdrianPerez/cmpe_131/CMPE131Team6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AD308C-FF5E-CE42-B854-BB8EE3603123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BAD476-9C17-B04E-95F1-BA13CEB777EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,9 +156,6 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>Feature 17</t>
-  </si>
-  <si>
     <t>Feature 18</t>
   </si>
   <si>
@@ -232,6 +229,9 @@
   </si>
   <si>
     <t>Filtering inbox</t>
+  </si>
+  <si>
+    <t>Register</t>
   </si>
 </sst>
 </file>
@@ -639,6 +639,30 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="3" applyBorder="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="7" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="7" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="6" borderId="10" xfId="13" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -686,30 +710,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="3" applyBorder="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="7" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="7" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="6" borderId="10" xfId="13" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1123,7 +1123,7 @@
   <dimension ref="B1:BO30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1148,13 +1148,13 @@
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1162,66 +1162,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="31"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="39"/>
       <c r="P2" s="16"/>
-      <c r="Q2" s="29" t="s">
+      <c r="Q2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="31"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="39"/>
       <c r="U2" s="17"/>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="33"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="41"/>
       <c r="Z2" s="18"/>
-      <c r="AA2" s="34" t="s">
+      <c r="AA2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="36"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="43"/>
+      <c r="AF2" s="43"/>
+      <c r="AG2" s="44"/>
       <c r="AH2" s="19"/>
-      <c r="AI2" s="21" t="s">
+      <c r="AI2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="22"/>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="22"/>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22"/>
-      <c r="AO2" s="22"/>
-      <c r="AP2" s="22"/>
+      <c r="AJ2" s="30"/>
+      <c r="AK2" s="30"/>
+      <c r="AL2" s="30"/>
+      <c r="AM2" s="30"/>
+      <c r="AN2" s="30"/>
+      <c r="AO2" s="30"/>
+      <c r="AP2" s="30"/>
     </row>
     <row r="3" spans="2:67" s="11" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="36" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="20" t="s">
@@ -1248,16 +1248,16 @@
       <c r="AA3" s="10"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="25"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="37">
+      <c r="B4" s="33"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="21">
         <v>1</v>
       </c>
-      <c r="I4" s="37">
+      <c r="I4" s="21">
         <v>2</v>
       </c>
       <c r="J4" s="3">
@@ -1437,7 +1437,7 @@
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1454,8 +1454,8 @@
       <c r="G5" s="8">
         <v>1</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="41"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="25"/>
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
@@ -1494,7 +1494,7 @@
       <c r="G6" s="8">
         <v>0</v>
       </c>
-      <c r="H6" s="39"/>
+      <c r="H6" s="23"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
@@ -1534,7 +1534,7 @@
       <c r="G7" s="8">
         <v>0</v>
       </c>
-      <c r="H7" s="42"/>
+      <c r="H7" s="26"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="7">
         <v>2</v>
@@ -1569,12 +1569,12 @@
         <v>2</v>
       </c>
       <c r="F8" s="7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G8" s="8">
         <v>0.75</v>
       </c>
-      <c r="H8" s="40"/>
+      <c r="H8" s="24"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="7">
         <v>2</v>
@@ -1614,7 +1614,7 @@
       <c r="G9" s="8">
         <v>0</v>
       </c>
-      <c r="H9" s="40"/>
+      <c r="H9" s="24"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="7">
         <v>8</v>
@@ -1654,8 +1654,8 @@
       <c r="G10" s="8">
         <v>0</v>
       </c>
-      <c r="H10" s="42"/>
-      <c r="I10" s="44"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="28"/>
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10"/>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="7">
         <v>12</v>
@@ -1694,7 +1694,7 @@
       <c r="G11" s="8">
         <v>0</v>
       </c>
-      <c r="H11" s="40"/>
+      <c r="H11" s="24"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="7">
         <v>12</v>
@@ -1734,7 +1734,7 @@
       <c r="G12" s="8">
         <v>0</v>
       </c>
-      <c r="H12" s="40"/>
+      <c r="H12" s="24"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1757,7 +1757,7 @@
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="7">
         <v>12</v>
@@ -1774,7 +1774,7 @@
       <c r="G13" s="8">
         <v>0</v>
       </c>
-      <c r="H13" s="40"/>
+      <c r="H13" s="24"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="7">
         <v>18</v>
@@ -1814,7 +1814,7 @@
       <c r="G14" s="8">
         <v>0</v>
       </c>
-      <c r="H14" s="40"/>
+      <c r="H14" s="24"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1837,7 +1837,7 @@
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="7">
         <v>18</v>
@@ -1854,7 +1854,7 @@
       <c r="G15" s="8">
         <v>0</v>
       </c>
-      <c r="H15" s="40"/>
+      <c r="H15" s="24"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="7">
         <v>18</v>
@@ -1894,7 +1894,7 @@
       <c r="G16" s="8">
         <v>0</v>
       </c>
-      <c r="H16" s="40"/>
+      <c r="H16" s="24"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="17" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="7">
         <v>18</v>
@@ -1934,7 +1934,7 @@
       <c r="G17" s="8">
         <v>0</v>
       </c>
-      <c r="H17" s="40"/>
+      <c r="H17" s="24"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1957,7 +1957,7 @@
     </row>
     <row r="18" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="7">
         <v>24</v>
@@ -1974,7 +1974,7 @@
       <c r="G18" s="8">
         <v>0</v>
       </c>
-      <c r="H18" s="40"/>
+      <c r="H18" s="24"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="19" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="7">
         <v>24</v>
@@ -2014,7 +2014,7 @@
       <c r="G19" s="8">
         <v>0</v>
       </c>
-      <c r="H19" s="40"/>
+      <c r="H19" s="24"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="20" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="7">
         <v>24</v>
@@ -2054,7 +2054,7 @@
       <c r="G20" s="8">
         <v>0</v>
       </c>
-      <c r="H20" s="40"/>
+      <c r="H20" s="24"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -2076,25 +2076,25 @@
       <c r="AA20"/>
     </row>
     <row r="21" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="43" t="s">
-        <v>15</v>
+      <c r="B21" s="27" t="s">
+        <v>40</v>
       </c>
       <c r="C21" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D21" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E21" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G21" s="8">
-        <v>0</v>
-      </c>
-      <c r="H21" s="40"/>
+        <v>1</v>
+      </c>
+      <c r="H21" s="24"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="22" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="7">
         <v>0</v>
@@ -2134,7 +2134,7 @@
       <c r="G22" s="8">
         <v>0</v>
       </c>
-      <c r="H22" s="40"/>
+      <c r="H22" s="24"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2157,7 +2157,7 @@
     </row>
     <row r="23" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="7">
         <v>0</v>
@@ -2174,7 +2174,7 @@
       <c r="G23" s="8">
         <v>0</v>
       </c>
-      <c r="H23" s="40"/>
+      <c r="H23" s="24"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="24" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="7">
         <v>0</v>
@@ -2214,7 +2214,7 @@
       <c r="G24" s="8">
         <v>0</v>
       </c>
-      <c r="H24" s="40"/>
+      <c r="H24" s="24"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2237,7 +2237,7 @@
     </row>
     <row r="25" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="7">
         <v>0</v>
@@ -2254,7 +2254,7 @@
       <c r="G25" s="8">
         <v>0</v>
       </c>
-      <c r="H25" s="40"/>
+      <c r="H25" s="24"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2277,7 +2277,7 @@
     </row>
     <row r="26" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" s="7">
         <v>0</v>
@@ -2294,7 +2294,7 @@
       <c r="G26" s="8">
         <v>0</v>
       </c>
-      <c r="H26" s="40"/>
+      <c r="H26" s="24"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="27" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="7">
         <v>0</v>
@@ -2334,7 +2334,7 @@
       <c r="G27" s="8">
         <v>0</v>
       </c>
-      <c r="H27" s="40"/>
+      <c r="H27" s="24"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="28" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="7">
         <v>0</v>
@@ -2374,7 +2374,7 @@
       <c r="G28" s="8">
         <v>0</v>
       </c>
-      <c r="H28" s="40"/>
+      <c r="H28" s="24"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2397,7 +2397,7 @@
     </row>
     <row r="29" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="7">
         <v>0</v>
@@ -2414,7 +2414,7 @@
       <c r="G29" s="8">
         <v>0</v>
       </c>
-      <c r="H29" s="40"/>
+      <c r="H29" s="24"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2437,7 +2437,7 @@
     </row>
     <row r="30" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="7">
         <v>0</v>
@@ -2454,7 +2454,7 @@
       <c r="G30" s="8">
         <v>0</v>
       </c>
-      <c r="H30" s="40"/>
+      <c r="H30" s="24"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>

</xml_diff>

<commit_message>
Modified gantt chart part 2 lol
</commit_message>
<xml_diff>
--- a/Taskr_gantt.xlsx
+++ b/Taskr_gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdrianPerez/cmpe_131/CMPE131Team6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F694AB5-9245-A244-8B00-6159CDD1F478}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98ED34FF-6657-8B47-9E34-19BF9CAD5851}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1129,7 +1129,7 @@
   <dimension ref="B1:BO30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1498,7 +1498,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6"/>
@@ -1578,7 +1578,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="8">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H8" s="24"/>
       <c r="I8"/>

</xml_diff>